<commit_message>
update order_new address function 20251119_jkk
</commit_message>
<xml_diff>
--- a/스프링부트 미니프로젝트_prontend_v20251117.xlsx
+++ b/스프링부트 미니프로젝트_prontend_v20251117.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="팀프로젝트" sheetId="6" r:id="rId1"/>
@@ -13,6 +13,9 @@
     <sheet name="요구사항 정리" sheetId="3" r:id="rId4"/>
     <sheet name="일정관리" sheetId="4" r:id="rId5"/>
     <sheet name="이력관리" sheetId="5" r:id="rId6"/>
+    <sheet name="객체" sheetId="7" r:id="rId7"/>
+    <sheet name="기능" sheetId="9" r:id="rId8"/>
+    <sheet name="진행사항" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">일정관리!$A$1:$AF$23</definedName>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="460">
   <si>
     <t>공통 API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1425,6 +1428,338 @@
   </si>
   <si>
     <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>객체명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CartVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OrderVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CropVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작물 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InventoryVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>창고 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShopVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상점 관련 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>myFarm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountServiceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressServiceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Command</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountRestController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddressRestController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommonController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OrderMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserSErviceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Util</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interceptor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginCheckInterceptor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sAdminCropMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminCropService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminCropServiceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inventory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InventoryMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InventoryService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InventoryServiceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminShopMapper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminShopService</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdminShopServiceImpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중분류-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중분류-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인화면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품을 진열한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dummy page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입을 한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자/관리자로 로그인을 한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자/관리자로 로그아웃을 한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4073,8 +4408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="A18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6064,7 +6399,7 @@
   <dimension ref="B3:X29"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8013,4 +8348,496 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5" t="s">
+        <v>394</v>
+      </c>
+      <c r="E5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8" t="s">
+        <v>391</v>
+      </c>
+      <c r="C8" t="s">
+        <v>392</v>
+      </c>
+      <c r="D8" t="s">
+        <v>393</v>
+      </c>
+      <c r="E8" t="s">
+        <v>394</v>
+      </c>
+      <c r="F8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C9" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" t="s">
+        <v>397</v>
+      </c>
+      <c r="E9" t="s">
+        <v>394</v>
+      </c>
+      <c r="F9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>399</v>
+      </c>
+      <c r="C10" t="s">
+        <v>400</v>
+      </c>
+      <c r="D10" t="s">
+        <v>397</v>
+      </c>
+      <c r="E10" t="s">
+        <v>394</v>
+      </c>
+      <c r="F10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="5" width="22.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>406</v>
+      </c>
+      <c r="I3" t="s">
+        <v>427</v>
+      </c>
+      <c r="J3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>407</v>
+      </c>
+      <c r="I4" t="s">
+        <v>429</v>
+      </c>
+      <c r="J4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>408</v>
+      </c>
+      <c r="E5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>412</v>
+      </c>
+      <c r="E8" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>414</v>
+      </c>
+      <c r="E16" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>421</v>
+      </c>
+      <c r="E22" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>431</v>
+      </c>
+      <c r="E26" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>435</v>
+      </c>
+      <c r="E29" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>439</v>
+      </c>
+      <c r="E32" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>442</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="9" style="12"/>
+    <col min="5" max="5" width="28.125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9" style="12"/>
+    <col min="7" max="7" width="13.375" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D9" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>